<commit_message>
2 api's module [async, semaphored]
</commit_message>
<xml_diff>
--- a/comparison_results.xlsx
+++ b/comparison_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>match</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>refresh_status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -470,6 +475,11 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -486,6 +496,11 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -502,6 +517,11 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -518,6 +538,11 @@
       <c r="D5" t="b">
         <v>0</v>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -534,6 +559,11 @@
       <c r="D6" t="b">
         <v>0</v>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -550,6 +580,11 @@
       <c r="D7" t="b">
         <v>0</v>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -566,6 +601,11 @@
       <c r="D8" t="b">
         <v>1</v>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -582,6 +622,11 @@
       <c r="D9" t="b">
         <v>0</v>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -598,6 +643,11 @@
       <c r="D10" t="b">
         <v>1</v>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -614,6 +664,11 @@
       <c r="D11" t="b">
         <v>0</v>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -630,6 +685,11 @@
       <c r="D12" t="b">
         <v>1</v>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -646,6 +706,11 @@
       <c r="D13" t="b">
         <v>0</v>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -662,6 +727,11 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -678,6 +748,11 @@
       <c r="D15" t="b">
         <v>0</v>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -689,10 +764,15 @@
         <v>12.75</v>
       </c>
       <c r="C16" t="n">
-        <v>12.75</v>
+        <v>13.75</v>
       </c>
       <c r="D16" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -705,10 +785,15 @@
         <v>12.751</v>
       </c>
       <c r="C17" t="n">
-        <v>12.75</v>
+        <v>13.75</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -726,6 +811,11 @@
       <c r="D18" t="b">
         <v>1</v>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -742,6 +832,11 @@
       <c r="D19" t="b">
         <v>0</v>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -758,6 +853,11 @@
       <c r="D20" t="b">
         <v>1</v>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -774,6 +874,11 @@
       <c r="D21" t="b">
         <v>0</v>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -790,6 +895,11 @@
       <c r="D22" t="b">
         <v>1</v>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -806,6 +916,11 @@
       <c r="D23" t="b">
         <v>0</v>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -822,6 +937,11 @@
       <c r="D24" t="b">
         <v>1</v>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -838,6 +958,11 @@
       <c r="D25" t="b">
         <v>0</v>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -854,6 +979,11 @@
       <c r="D26" t="b">
         <v>1</v>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -870,6 +1000,11 @@
       <c r="D27" t="b">
         <v>0</v>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -886,6 +1021,11 @@
       <c r="D28" t="b">
         <v>1</v>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -902,6 +1042,11 @@
       <c r="D29" t="b">
         <v>0</v>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -918,6 +1063,11 @@
       <c r="D30" t="b">
         <v>1</v>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -934,6 +1084,11 @@
       <c r="D31" t="b">
         <v>0</v>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -950,6 +1105,11 @@
       <c r="D32" t="b">
         <v>1</v>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -966,6 +1126,11 @@
       <c r="D33" t="b">
         <v>0</v>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -982,6 +1147,11 @@
       <c r="D34" t="b">
         <v>1</v>
       </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -998,6 +1168,11 @@
       <c r="D35" t="b">
         <v>0</v>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1014,6 +1189,11 @@
       <c r="D36" t="b">
         <v>1</v>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1030,6 +1210,11 @@
       <c r="D37" t="b">
         <v>0</v>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1046,6 +1231,11 @@
       <c r="D38" t="b">
         <v>1</v>
       </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1062,6 +1252,11 @@
       <c r="D39" t="b">
         <v>0</v>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1078,6 +1273,11 @@
       <c r="D40" t="b">
         <v>1</v>
       </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1094,6 +1294,11 @@
       <c r="D41" t="b">
         <v>0</v>
       </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1110,6 +1315,11 @@
       <c r="D42" t="b">
         <v>1</v>
       </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1126,6 +1336,11 @@
       <c r="D43" t="b">
         <v>0</v>
       </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1142,6 +1357,11 @@
       <c r="D44" t="b">
         <v>1</v>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1158,6 +1378,11 @@
       <c r="D45" t="b">
         <v>0</v>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1174,6 +1399,11 @@
       <c r="D46" t="b">
         <v>1</v>
       </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1190,6 +1420,11 @@
       <c r="D47" t="b">
         <v>0</v>
       </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1206,6 +1441,11 @@
       <c r="D48" t="b">
         <v>1</v>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1222,6 +1462,11 @@
       <c r="D49" t="b">
         <v>0</v>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1238,6 +1483,11 @@
       <c r="D50" t="b">
         <v>1</v>
       </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1254,6 +1504,11 @@
       <c r="D51" t="b">
         <v>0</v>
       </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1270,6 +1525,11 @@
       <c r="D52" t="b">
         <v>1</v>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1285,6 +1545,11 @@
       </c>
       <c r="D53" t="b">
         <v>0</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>